<commit_message>
update code and excel
</commit_message>
<xml_diff>
--- a/methods_list.xlsx
+++ b/methods_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tfigueiredo/Documents/ISEC/4A_1S/PD/API_REST_PD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30BD7D9-9D6F-DE4B-A934-DCC6B207C4FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC303D8-3042-3B4D-BBC0-3873AB836B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11980" yWindow="1560" windowWidth="23040" windowHeight="19100" xr2:uid="{8DEBF184-A62F-1A4C-91C2-55E3BFEA1652}"/>
+    <workbookView xWindow="720" yWindow="500" windowWidth="33600" windowHeight="19580" xr2:uid="{8DEBF184-A62F-1A4C-91C2-55E3BFEA1652}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="64">
   <si>
     <t>GET</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>REQUEST BODY</t>
-  </si>
-  <si>
-    <t>RESPONSE BODY</t>
   </si>
   <si>
     <t>POST</t>
@@ -135,9 +132,6 @@
     <t>Submeter o código associado a um evento para efeitos de registo da presença.</t>
   </si>
   <si>
-    <t>/submit</t>
-  </si>
-  <si>
     <t>USER</t>
   </si>
   <si>
@@ -176,25 +170,10 @@
     <t>Devolve uma listagem de todos os eventos em que o utilizador tem presença marcada.</t>
   </si>
   <si>
-    <t>/attendances/{eventName}</t>
-  </si>
-  <si>
-    <t>/attendances/{eventDate}</t>
-  </si>
-  <si>
-    <t>/attendances/{eventLocal}</t>
-  </si>
-  <si>
     <t>{"name"="Event Name"}</t>
   </si>
   <si>
-    <t>{"dateSTART":"2023-01-01", "dateEND":"2023-02-01"}</t>
-  </si>
-  <si>
     <t>{"code":"AXA435"}</t>
-  </si>
-  <si>
-    <t>{"local":"ISEC"}</t>
   </si>
   <si>
     <t>-</t>
@@ -249,19 +228,7 @@
     </r>
   </si>
   <si>
-    <t>{"id":"1"}</t>
-  </si>
-  <si>
-    <t>200 - OK (eliminou - vem o objeto que foi eliminado) 400 - erro (vem info a dizer que o evento já tem presenças registadas)</t>
-  </si>
-  <si>
     <t>/events/{eventId}</t>
-  </si>
-  <si>
-    <t>/events/{eventDate}</t>
-  </si>
-  <si>
-    <t>/events/{eventLocal}</t>
   </si>
   <si>
     <r>
@@ -293,16 +260,10 @@
     <t>Devolve uma listagem de todos os eventos em que ocorram durante essa data.</t>
   </si>
   <si>
-    <t>/events/{eventName}</t>
-  </si>
-  <si>
     <t>Devolve uma listagem de todos os eventos cujo nome foi pedido.</t>
   </si>
   <si>
     <t>/attendances/{eventID}</t>
-  </si>
-  <si>
-    <t>PUT</t>
   </si>
   <si>
     <r>
@@ -353,6 +314,60 @@
   </si>
   <si>
     <t>Devolve uma listagem de todos os utilzadores registados no envento cujo ID foi pedido.</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>/events?{eventName}</t>
+  </si>
+  <si>
+    <t>/events?{eventLocal}</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>REQUEST PARAMETERS</t>
+  </si>
+  <si>
+    <t>/attendances?{eventName}</t>
+  </si>
+  <si>
+    <t>/attendances?{eventLocal}</t>
+  </si>
+  <si>
+    <t>ver como faço para poder usar dois construtures no evento (e deixar de usar o userconfig e passar a usar o User com 2 construtores)</t>
+  </si>
+  <si>
+    <t>PATCH</t>
+  </si>
+  <si>
+    <t>dados que quero alterar</t>
+  </si>
+  <si>
+    <t>/attendances?{eventDateStart}&amp;{eventDateEnd}</t>
+  </si>
+  <si>
+    <t>/events?{eventDateStart}&amp;{eventDateEnd}</t>
+  </si>
+  <si>
+    <t>{"startDate":"2023-01-01", "endDate":"2023-02-01"}</t>
+  </si>
+  <si>
+    <t>{"location":"ISEC"}</t>
+  </si>
+  <si>
+    <t>{"name":"Ze dos leitoes", "location":"ISEC", "date":"2023-11-19", "startTime":"15:30", "endTime":"19:30"}</t>
+  </si>
+  <si>
+    <t>/events/{eventID}</t>
+  </si>
+  <si>
+    <t>melhorar por causa do ID</t>
+  </si>
+  <si>
+    <t>meter a verificação temporal a funcionar</t>
   </si>
 </sst>
 </file>
@@ -510,14 +525,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -551,54 +560,60 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -608,26 +623,21 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -949,435 +959,514 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0F7FF9E-169B-9C4B-9827-0D41174D787B}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="34.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="41.33203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="33.6640625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="30.83203125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="38.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="33.5" style="3" customWidth="1"/>
+    <col min="7" max="7" width="30.83203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="33.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="30"/>
+      <c r="B3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="35"/>
+    </row>
+    <row r="5" spans="1:10" ht="67" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="30"/>
+      <c r="B6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="31"/>
+      <c r="F6" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="30"/>
+      <c r="B7" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="31"/>
+      <c r="F7" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="30"/>
+      <c r="B8" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="31"/>
+      <c r="F8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="30"/>
+      <c r="B9" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="31"/>
+      <c r="F9" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="30"/>
+      <c r="B10" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="20"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="35"/>
+      <c r="J10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="30"/>
+      <c r="B11" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="J11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="30"/>
+      <c r="B12" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="I12" s="35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="35"/>
+    </row>
+    <row r="14" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I14" s="35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="30"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="35"/>
+    </row>
+    <row r="16" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="30"/>
+      <c r="B16" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="J16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="30"/>
+      <c r="B17" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="30"/>
+      <c r="B18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="D18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="33"/>
+      <c r="F18" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H18" s="6"/>
+      <c r="I18" s="35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="30"/>
+      <c r="B19" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="41"/>
-    </row>
-    <row r="3" spans="1:8" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="36"/>
-      <c r="B3" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="G3" s="37" t="s">
-        <v>54</v>
-      </c>
-      <c r="H3" s="18"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="15"/>
-    </row>
-    <row r="5" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="36" t="s">
+      <c r="C19" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="33"/>
+      <c r="F19" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H19" s="6"/>
+      <c r="I19" s="35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="30"/>
+      <c r="B20" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" s="7"/>
-    </row>
-    <row r="6" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="36"/>
-      <c r="B6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="H6" s="7"/>
-    </row>
-    <row r="7" spans="1:8" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="36"/>
-      <c r="B7" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G7" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="7"/>
-    </row>
-    <row r="8" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="36"/>
-      <c r="B8" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="36"/>
-      <c r="B9" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9" s="41"/>
-    </row>
-    <row r="10" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="36"/>
-      <c r="B10" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="23" t="s">
+      <c r="D20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="34"/>
+      <c r="F20" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="H20" s="6"/>
+      <c r="I20" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="F10" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="H10" s="22"/>
-    </row>
-    <row r="11" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="36"/>
-      <c r="B11" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="G11" s="20"/>
-      <c r="H11" s="18"/>
-    </row>
-    <row r="12" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="36"/>
-      <c r="B12" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="H12" s="26" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="15"/>
-    </row>
-    <row r="14" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="G14" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="H14" s="18"/>
-    </row>
-    <row r="15" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="38" t="s">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G16" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="H16" s="7"/>
-    </row>
-    <row r="17" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="39"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="39"/>
-      <c r="B18" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="H18" s="7"/>
-    </row>
-    <row r="19" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="39"/>
-      <c r="B19" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="33"/>
-      <c r="F19" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G19" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="H19" s="7"/>
-    </row>
-    <row r="20" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="39"/>
-      <c r="B20" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E20" s="33"/>
-      <c r="F20" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="H20" s="7"/>
-    </row>
-    <row r="21" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="40"/>
-      <c r="B21" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" s="34"/>
-      <c r="F21" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G21" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="H21" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A5:A12"/>
-    <mergeCell ref="A16:A21"/>
     <mergeCell ref="E5:E9"/>
-    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="E17:E20"/>
+    <mergeCell ref="A14:A20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[UI] menus working, tests InProg.
</commit_message>
<xml_diff>
--- a/methods_list.xlsx
+++ b/methods_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tfigueiredo/Documents/ISEC/4A_1S/PD/API_REST_PD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC303D8-3042-3B4D-BBC0-3873AB836B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1103B6FE-C8D4-FE4F-9154-CD6670AA91FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="500" windowWidth="33600" windowHeight="19580" xr2:uid="{8DEBF184-A62F-1A4C-91C2-55E3BFEA1652}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20180" xr2:uid="{8DEBF184-A62F-1A4C-91C2-55E3BFEA1652}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="67">
   <si>
     <t>GET</t>
   </si>
@@ -266,6 +266,9 @@
     <t>/attendances/{eventID}</t>
   </si>
   <si>
+    <t>PUT</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -316,9 +319,6 @@
     <t>Devolve uma listagem de todos os utilzadores registados no envento cujo ID foi pedido.</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>/events?{eventName}</t>
   </si>
   <si>
@@ -337,15 +337,6 @@
     <t>/attendances?{eventLocal}</t>
   </si>
   <si>
-    <t>ver como faço para poder usar dois construtures no evento (e deixar de usar o userconfig e passar a usar o User com 2 construtores)</t>
-  </si>
-  <si>
-    <t>PATCH</t>
-  </si>
-  <si>
-    <t>dados que quero alterar</t>
-  </si>
-  <si>
     <t>/attendances?{eventDateStart}&amp;{eventDateEnd}</t>
   </si>
   <si>
@@ -364,17 +355,35 @@
     <t>/events/{eventID}</t>
   </si>
   <si>
-    <t>melhorar por causa do ID</t>
-  </si>
-  <si>
-    <t>meter a verificação temporal a funcionar</t>
+    <t>{"timeout":10}</t>
+  </si>
+  <si>
+    <t>Devolve uma listagem de todos as presenças cujo evento tenha o nome pedido.</t>
+  </si>
+  <si>
+    <t>Devolve uma listagem de todos as presenças cujos eventos ocorram nessa data.</t>
+  </si>
+  <si>
+    <t>Devolve uma listagem de todos as presenças cujos eventos ocorrem nesse local.</t>
+  </si>
+  <si>
+    <t>Devolve o respetivo evento com o código gerado.</t>
+  </si>
+  <si>
+    <t>TESTAR A DURAÇÃO DO TOKEN</t>
+  </si>
+  <si>
+    <t>TEST NOK</t>
+  </si>
+  <si>
+    <t>TEST OK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -422,6 +431,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -461,7 +486,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -521,11 +546,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -572,6 +606,9 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -623,9 +660,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -636,8 +670,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -959,13 +995,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0F7FF9E-169B-9C4B-9827-0D41174D787B}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
@@ -975,11 +1011,12 @@
     <col min="6" max="6" width="33.5" style="3" customWidth="1"/>
     <col min="7" max="7" width="30.83203125" style="3" customWidth="1"/>
     <col min="8" max="8" width="33.6640625" style="2" customWidth="1"/>
+    <col min="9" max="10" width="10.83203125" style="42"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
@@ -1002,9 +1039,16 @@
       <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="30" t="s">
+      <c r="I1" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" s="41"/>
+    </row>
+    <row r="2" spans="1:11" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1028,12 +1072,15 @@
       <c r="H2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="35" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="30"/>
+      <c r="I2" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" s="40" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="31"/>
       <c r="B3" s="15" t="s">
         <v>6</v>
       </c>
@@ -1046,20 +1093,17 @@
       <c r="E3" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" s="29" t="s">
+      <c r="F3" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="30" t="s">
         <v>26</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="I3" s="35" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
@@ -1067,11 +1111,10 @@
       <c r="F4" s="13"/>
       <c r="G4" s="38"/>
       <c r="H4" s="12"/>
-      <c r="I4" s="35"/>
-    </row>
-    <row r="5" spans="1:10" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="30" t="s">
-        <v>39</v>
+    </row>
+    <row r="5" spans="1:11" ht="67" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="31" t="s">
+        <v>40</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>0</v>
@@ -1079,10 +1122,10 @@
       <c r="C5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="32" t="s">
         <v>31</v>
       </c>
       <c r="F5" s="14" t="s">
@@ -1094,22 +1137,19 @@
       <c r="H5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="35" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="30"/>
+    </row>
+    <row r="6" spans="1:11" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="31"/>
       <c r="B6" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="31"/>
+      <c r="E6" s="32"/>
       <c r="F6" s="14" t="s">
         <v>26</v>
       </c>
@@ -1119,22 +1159,19 @@
       <c r="H6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="35" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="30"/>
+    </row>
+    <row r="7" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="31"/>
       <c r="B7" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="31"/>
+      <c r="E7" s="32"/>
       <c r="F7" s="14" t="s">
         <v>26</v>
       </c>
@@ -1144,142 +1181,131 @@
       <c r="H7" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="35" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="30"/>
+    </row>
+    <row r="8" spans="1:11" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="31"/>
       <c r="B8" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="31"/>
+      <c r="E8" s="32"/>
       <c r="F8" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="I8" s="35" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="30"/>
+    </row>
+    <row r="9" spans="1:11" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="31"/>
       <c r="B9" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="31"/>
+      <c r="E9" s="32"/>
       <c r="F9" s="14" t="s">
         <v>26</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="35" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="30"/>
-      <c r="B10" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" s="18" t="s">
+    </row>
+    <row r="10" spans="1:11" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="31"/>
+      <c r="B10" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="G10" s="20"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="35"/>
-      <c r="J10" t="s">
+      <c r="E10" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10" s="21"/>
+      <c r="H10" s="20" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="30"/>
+      <c r="I10" s="42" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="31"/>
       <c r="B11" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="27" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="29" t="s">
-        <v>60</v>
+      <c r="F11" s="30" t="s">
+        <v>57</v>
       </c>
       <c r="G11" s="17" t="s">
         <v>26</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="I11" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="I11" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="J11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="30"/>
-      <c r="B12" s="21" t="s">
+    </row>
+    <row r="12" spans="1:11" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="31"/>
+      <c r="B12" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" s="27" t="s">
+      <c r="C12" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="I12" s="35" t="s">
+      <c r="F12" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="I12" s="42" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
@@ -1287,11 +1313,10 @@
       <c r="F13" s="13"/>
       <c r="G13" s="38"/>
       <c r="H13" s="12"/>
-      <c r="I13" s="35"/>
-    </row>
-    <row r="14" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="30" t="s">
-        <v>40</v>
+    </row>
+    <row r="14" spans="1:11" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="31" t="s">
+        <v>41</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>0</v>
@@ -1299,11 +1324,11 @@
       <c r="C14" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="24" t="s">
+      <c r="D14" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="28" t="s">
-        <v>37</v>
+      <c r="E14" s="29" t="s">
+        <v>38</v>
       </c>
       <c r="F14" s="14" t="s">
         <v>26</v>
@@ -1312,14 +1337,11 @@
         <v>26</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="I14" s="35" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="30"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="31"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -1327,40 +1349,36 @@
       <c r="F15" s="10"/>
       <c r="G15" s="39"/>
       <c r="H15" s="9"/>
-      <c r="I15" s="35"/>
-    </row>
-    <row r="16" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="30"/>
-      <c r="B16" s="18" t="s">
+    </row>
+    <row r="16" spans="1:11" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="31"/>
+      <c r="B16" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="40" t="s">
+      <c r="E16" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="20" t="s">
+      <c r="F16" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="H16" s="19" t="s">
+      <c r="G16" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="I16" s="35" t="s">
+      <c r="I16" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="J16" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="30"/>
+    </row>
+    <row r="17" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="31"/>
       <c r="B17" s="5" t="s">
         <v>0</v>
       </c>
@@ -1370,7 +1388,7 @@
       <c r="D17" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="32" t="s">
+      <c r="E17" s="33" t="s">
         <v>22</v>
       </c>
       <c r="F17" s="14" t="s">
@@ -1382,12 +1400,9 @@
       <c r="H17" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I17" s="35" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="30"/>
+    </row>
+    <row r="18" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="31"/>
       <c r="B18" s="5" t="s">
         <v>0</v>
       </c>
@@ -1397,43 +1412,41 @@
       <c r="D18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="33"/>
+      <c r="E18" s="34"/>
       <c r="F18" s="14" t="s">
         <v>26</v>
       </c>
       <c r="G18" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="H18" s="6"/>
-      <c r="I18" s="35" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="30"/>
+      <c r="H18" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="31"/>
       <c r="B19" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="33"/>
+      <c r="E19" s="34"/>
       <c r="F19" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="H19" s="6"/>
-      <c r="I19" s="35" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="30"/>
+        <v>55</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="31"/>
       <c r="B20" s="5" t="s">
         <v>0</v>
       </c>
@@ -1443,21 +1456,15 @@
       <c r="D20" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="34"/>
+      <c r="E20" s="35"/>
       <c r="F20" s="14" t="s">
         <v>26</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="H20" s="6"/>
-      <c r="I20" s="35" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>53</v>
+        <v>56</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>